<commit_message>
Paper: Plot EIA 860 capacity
</commit_message>
<xml_diff>
--- a/CreateDB_NC/InputData/ExcelUserData/UserDataPart3.xlsx
+++ b/CreateDB_NC/InputData/ExcelUserData/UserDataPart3.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor\Desktop\TEMOA\TemoaHurricane_V2\CreateDB_NC\InputData\ExcelUserData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Remote\Desktop\Projects\TemoaHurricane_OEA\TEMOA_GIT\TemoaHurricane_V2\CreateDB_NC\InputData\ExcelUserData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1365F7-ED3D-4E45-BACB-A36145F4249D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0381AB16-8636-4499-9321-A8B0B4433AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43080" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="groups" sheetId="1" r:id="rId1"/>
     <sheet name="MaxCapacityGroup" sheetId="2" r:id="rId2"/>
+    <sheet name="TechColor" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="139">
   <si>
     <t>Group Name</t>
   </si>
@@ -106,13 +107,361 @@
   </si>
   <si>
     <t>WAT_PS_EXISTING</t>
+  </si>
+  <si>
+    <t>Tech</t>
+  </si>
+  <si>
+    <t>Pallet</t>
+  </si>
+  <si>
+    <t>Idx</t>
+  </si>
+  <si>
+    <t>AB_ST_EXISTING</t>
+  </si>
+  <si>
+    <t>tab20b</t>
+  </si>
+  <si>
+    <t>BIT_ST_EXISTING</t>
+  </si>
+  <si>
+    <t>BLQ_ST_EXISTING</t>
+  </si>
+  <si>
+    <t>DFO_CC_EXISTING</t>
+  </si>
+  <si>
+    <t>DFO_GT_EXISTING</t>
+  </si>
+  <si>
+    <t>DFO_IC_EXISTING</t>
+  </si>
+  <si>
+    <t>LFG_GT_EXISTING</t>
+  </si>
+  <si>
+    <t>LFG_IC_EXISTING</t>
+  </si>
+  <si>
+    <t>MWH_BA1H_EXISTING</t>
+  </si>
+  <si>
+    <t>MWH_BA2H_EXISTING</t>
+  </si>
+  <si>
+    <t>NG_CC_EXISTING</t>
+  </si>
+  <si>
+    <t>NG_GT_EXISTING</t>
+  </si>
+  <si>
+    <t>NG_ST_EXISTING</t>
+  </si>
+  <si>
+    <t>NUC_ST_EXISTING</t>
+  </si>
+  <si>
+    <t>OBG_IC_EXISTING</t>
+  </si>
+  <si>
+    <t>SUN_PV_EXISTING</t>
+  </si>
+  <si>
+    <t>WDS_ST_EXISTING</t>
+  </si>
+  <si>
+    <t>WH_ST_EXISTING</t>
+  </si>
+  <si>
+    <t>WND_WT_EXISTING</t>
+  </si>
+  <si>
+    <t>BATT_2H_NEW</t>
+  </si>
+  <si>
+    <t>BATT_4H_NEW</t>
+  </si>
+  <si>
+    <t>BATT_6H_NEW</t>
+  </si>
+  <si>
+    <t>BATT_8H_NEW</t>
+  </si>
+  <si>
+    <t>BIOMASS_CC90_NEW</t>
+  </si>
+  <si>
+    <t>BIOMASS_NEW</t>
+  </si>
+  <si>
+    <t>COAL_95CC_NEW</t>
+  </si>
+  <si>
+    <t>COAL_99CC_NEW</t>
+  </si>
+  <si>
+    <t>COAL_NEW</t>
+  </si>
+  <si>
+    <t>NG_F-FRAME_CC_95CC_NEW</t>
+  </si>
+  <si>
+    <t>NG_F-FRAME_CC_97CC_NEW</t>
+  </si>
+  <si>
+    <t>NG_F-FRAME_CC_NEW</t>
+  </si>
+  <si>
+    <t>NG_F-FRAME_CT_NEW</t>
+  </si>
+  <si>
+    <t>NG_H-FRAME_CC_95CC_NEW</t>
+  </si>
+  <si>
+    <t>NG_H-FRAME_CC_97CC_NEW</t>
+  </si>
+  <si>
+    <t>NG_H-FRAME_CC_NEW</t>
+  </si>
+  <si>
+    <t>NUCLEAR-AP1000_NEW</t>
+  </si>
+  <si>
+    <t>NUCLEAR-SMR_NEW</t>
+  </si>
+  <si>
+    <t>PV-COMMERCIAL_NEW</t>
+  </si>
+  <si>
+    <t>PV-RESIDENTIAL_NEW</t>
+  </si>
+  <si>
+    <t>PV-UTILITY_NEW</t>
+  </si>
+  <si>
+    <t>WIND-LAND-C8_NEW</t>
+  </si>
+  <si>
+    <t>WIND-OFFSHORE-C6_NEW</t>
+  </si>
+  <si>
+    <t>CO2_STORAGE</t>
+  </si>
+  <si>
+    <t>DISTRIBUTION</t>
+  </si>
+  <si>
+    <t>FT_BIOMASS</t>
+  </si>
+  <si>
+    <t>FT_COAL</t>
+  </si>
+  <si>
+    <t>FT_NG</t>
+  </si>
+  <si>
+    <t>FT_NUCLEAR</t>
+  </si>
+  <si>
+    <t>FT_PETROLEUM</t>
+  </si>
+  <si>
+    <t>TRANSMISSION_INTERREGIONAL</t>
+  </si>
+  <si>
+    <t>TRANSMISSION_REGIONAL</t>
+  </si>
+  <si>
+    <t>Tech Description</t>
+  </si>
+  <si>
+    <t>Steam Turbine Using Agricultural By-Products (EIA 860 Nomenclature)</t>
+  </si>
+  <si>
+    <t>Steam Turbine Using Bituminous Coal (EIA 860 Nomenclature)</t>
+  </si>
+  <si>
+    <t>Steam Turbine Using Black Liquor (EIA 860 Nomenclature)</t>
+  </si>
+  <si>
+    <t>Combined Cycle Combustion Turbine Using Petroleum (EIA 860 Nomenclature)</t>
+  </si>
+  <si>
+    <t>Combustion Turbine Using Petroleum (EIA 860 Nomenclature)</t>
+  </si>
+  <si>
+    <t>Internal Combustion Engine Using Petroleum (EIA 860 Nomenclature)</t>
+  </si>
+  <si>
+    <t>Combustion Turbine Using Landfill Gas (EIA 860 Nomenclature)</t>
+  </si>
+  <si>
+    <t>Internal Combustion Engine Using Landfill Gas (EIA 860 Nomenclature)</t>
+  </si>
+  <si>
+    <t>Battery  Storage- 1h  (EIA 860 Nomenclature)</t>
+  </si>
+  <si>
+    <t>Battery  Storage- 2h  (EIA 860 Nomenclature)</t>
+  </si>
+  <si>
+    <t>Combined Cycle Combustion Turbine Using Natural Gas (EIA 860 Nomenclature)</t>
+  </si>
+  <si>
+    <t>Combustion Turbine Using Natural Gas (EIA 860 Nomenclature)</t>
+  </si>
+  <si>
+    <t>Steam Turbine Using Natural Gas (EIA 860 Nomenclature)</t>
+  </si>
+  <si>
+    <t>Nuclear Turbine (EIA 860 Nomenclature)</t>
+  </si>
+  <si>
+    <t>Internal Combustion Engine Using Other Biomass Gas (EIA 860 Nomenclature)</t>
+  </si>
+  <si>
+    <t>Solar Photovoltaic - Utility (EIA 860 Nomenclature)</t>
+  </si>
+  <si>
+    <t>Conventional Hydroelectric (EIA 860 Nomenclature)</t>
+  </si>
+  <si>
+    <t>Hydroelectric Pumped Storage (EIA 860 Nomenclature)</t>
+  </si>
+  <si>
+    <t>Steam Turbine Using Wood Waste (EIA 860 Nomenclature)</t>
+  </si>
+  <si>
+    <t>Steam Turbine Using Waste Heat (EIA 860 Nomenclature)</t>
+  </si>
+  <si>
+    <t>Onshore Wind Turbine (EIA 860 Nomenclature)</t>
+  </si>
+  <si>
+    <t>Battery Storage 2h (NREL ATB 2023 Technology)</t>
+  </si>
+  <si>
+    <t>Battery Storage 4h (NREL ATB 2023 Technology)</t>
+  </si>
+  <si>
+    <t>Battery Storage 6h (NREL ATB 2023 Technology)</t>
+  </si>
+  <si>
+    <t>Battery Storage 8h (NREL ATB 2023 Technology)</t>
+  </si>
+  <si>
+    <t>Generation From Biomass With 90% Carbon Capture (Technology from NREL ReEDS model  Using BECC-mod)</t>
+  </si>
+  <si>
+    <t>Generation From Biomass (NREL ATB 2023 Technology)</t>
+  </si>
+  <si>
+    <t>Generation From Coal With 95% Carbon Capture (NREL ATB 2023 Technology)</t>
+  </si>
+  <si>
+    <t>Generation From Coal With 99% Carbon Capture (NREL ATB 2023 Technology)</t>
+  </si>
+  <si>
+    <t>Generation From Coal (NREL ATB 2023 Technology)</t>
+  </si>
+  <si>
+    <t>Combined Cycle Natural Gas Turbine F-Frame With 95 % of Carbon Capture (NREL ATB 2023 Technology)</t>
+  </si>
+  <si>
+    <t>Combined Cycle Natural Gas Turbine F-Frame With 97 % of Carbon Capture (NREL ATB 2023 Technology)</t>
+  </si>
+  <si>
+    <t>Combined Cycle Natural Gas Turbine F-Frame (NREL ATB 2023 Technology)</t>
+  </si>
+  <si>
+    <t>Natural Gas Combustion Turbine F-Frame - Simple Cycle (NREL ATB 2023 Technology)</t>
+  </si>
+  <si>
+    <t>Combined Cycle Natural Gas Turbine H-Frame With 95 % of Carbon Capture (NREL ATB 2023 Technology)</t>
+  </si>
+  <si>
+    <t>Combined Cycle Natural Gas Turbine H-Frame With 97 % of Carbon Capture (NREL ATB 2023 Technology)</t>
+  </si>
+  <si>
+    <t>Combined Cycle Natural Gas Turbine H-Frame (NREL ATB 2023 Technology)</t>
+  </si>
+  <si>
+    <t>Nuclear Generation Using AP1000 PWR (NREL ATB 2023 Technology)</t>
+  </si>
+  <si>
+    <t>Small Modular Nuclear Reactor (NREL ATB 2023 Technology)</t>
+  </si>
+  <si>
+    <t>Commercial Solar PV (NREL ATB 2023 Technology)</t>
+  </si>
+  <si>
+    <t>Residential Solar PV (NREL ATB 2023 Technology)</t>
+  </si>
+  <si>
+    <t>Utility Solar PV (NREL ATB 2023 Technology)</t>
+  </si>
+  <si>
+    <t>Conventional Hydroelectric (NREL ATB 2023 Technology)</t>
+  </si>
+  <si>
+    <t>Hydroelectric Pumped Storage (NREL ATB 2023 Technology)</t>
+  </si>
+  <si>
+    <t>Onshore Wind Turbine Class 8 From NREL ATB 2023  (NREL ATB 2023 Technology)</t>
+  </si>
+  <si>
+    <t>Offshore Wind Turbine Class 6 From NREL ATB 2023  (NREL ATB 2023 Technology)</t>
+  </si>
+  <si>
+    <t>CO2 Storage</t>
+  </si>
+  <si>
+    <t>Energy Distribution</t>
+  </si>
+  <si>
+    <t>Fuel for Generation Technologies that Use Biomass</t>
+  </si>
+  <si>
+    <t>Fuel for Generation Technologies that Use Coal</t>
+  </si>
+  <si>
+    <t>Fuel for Generation Technologies that Use Natural Gas</t>
+  </si>
+  <si>
+    <t>Fuel for Nuclear Generation Technologies</t>
+  </si>
+  <si>
+    <t>Fuel for Generation Technologies that Use Petroleum</t>
+  </si>
+  <si>
+    <t>Transmission Between Different Regions</t>
+  </si>
+  <si>
+    <t>Transmission In the Same Region</t>
+  </si>
+  <si>
+    <t>tab20c</t>
+  </si>
+  <si>
+    <t>tab20</t>
+  </si>
+  <si>
+    <t>Set3</t>
+  </si>
+  <si>
+    <t>Paired</t>
+  </si>
+  <si>
+    <t>tab10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,13 +475,69 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3399"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -147,17 +552,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF3399"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -512,7 +937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C5C9527-1881-4D6D-BD71-38E11E56DCAB}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -736,4 +1161,822 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB0F5A9-D905-4459-BBED-C585707C2B23}">
+  <dimension ref="A1:D61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="3" width="22.1328125" customWidth="1"/>
+    <col min="4" max="4" width="82.265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3" s="6">
+        <v>16</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="2">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" s="6">
+        <v>17</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C6" s="6">
+        <v>18</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C7" s="6">
+        <v>19</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="2">
+        <v>10</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="2">
+        <v>11</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10" s="7">
+        <v>18</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C11" s="7">
+        <v>19</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C12" s="8">
+        <v>4</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C13" s="8">
+        <v>5</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C14" s="8">
+        <v>6</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C15" s="8">
+        <v>7</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C16" s="2">
+        <v>10</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C17" s="9">
+        <v>11</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="C18" s="10">
+        <v>0</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="C19" s="10">
+        <v>1</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C20" s="2">
+        <v>11</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C21" s="11">
+        <v>11</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="C22" s="12">
+        <v>6</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A23" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="3">
+        <v>1</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A24" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="3">
+        <v>2</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A25" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="3">
+        <v>3</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A26" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="3">
+        <v>4</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="2">
+        <v>5</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="2">
+        <v>6</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A29" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="3">
+        <v>7</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A30" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="3">
+        <v>8</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A31" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="3">
+        <v>9</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A32" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="3">
+        <v>10</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A33" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="3">
+        <v>11</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A34" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="3">
+        <v>12</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A35" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" s="3">
+        <v>13</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A36" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" s="3">
+        <v>14</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A37" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C37" s="3">
+        <v>15</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A38" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" s="3">
+        <v>16</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A39" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C39" s="3">
+        <v>17</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A40" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C40" s="3">
+        <v>18</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A41" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" s="3">
+        <v>19</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A42" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C42" s="3">
+        <v>0</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A43" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C43" s="3">
+        <v>1</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A44" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C44" s="3">
+        <v>2</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A45" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C45" s="3">
+        <v>3</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A46" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C46" s="3">
+        <v>4</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A47" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C47" s="3">
+        <v>5</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A48" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C48" s="3">
+        <v>6</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A49" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C49" s="3">
+        <v>7</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A50" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C50" s="2">
+        <v>8</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A51" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C51" s="3">
+        <v>9</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A52" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C52" s="3">
+        <v>10</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A53" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C53" s="3">
+        <v>11</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A54" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C54" s="3">
+        <v>12</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A55" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C55" s="3">
+        <v>13</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A56" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C56" s="3">
+        <v>14</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C57" s="3"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C58" s="3"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C59" s="3"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C60" s="3"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C61" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Code for new Tech (dist Gen + Intechange) - ok run
</commit_message>
<xml_diff>
--- a/CreateDB_NC/InputData/ExcelUserData/UserDataPart3.xlsx
+++ b/CreateDB_NC/InputData/ExcelUserData/UserDataPart3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Remote\Desktop\Projects\TemoaHurricane_OEA\TEMOA_GIT\TemoaHurricane_V2\CreateDB_NC\InputData\ExcelUserData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534B844C-8D17-49D1-AEF1-CF55F93A1BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{528B3737-44F8-40F0-91F5-7723DB5ABBAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="groups" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="186">
   <si>
     <t>Group Name</t>
   </si>
@@ -444,9 +444,6 @@
     <t>tab20</t>
   </si>
   <si>
-    <t>Set3</t>
-  </si>
-  <si>
     <t>Paired</t>
   </si>
   <si>
@@ -574,6 +571,33 @@
   </si>
   <si>
     <t xml:space="preserve">Max Cap Values from NREL- wind analysis </t>
+  </si>
+  <si>
+    <t>PV-COMMERCIAL</t>
+  </si>
+  <si>
+    <t>PV-RESIDENTIAL</t>
+  </si>
+  <si>
+    <t>GENERAL_CO2_CAP</t>
+  </si>
+  <si>
+    <t>ENERGY_INTERCHANGE</t>
+  </si>
+  <si>
+    <t>Tech Used to Represent Other Options For CO2 Capture</t>
+  </si>
+  <si>
+    <t>Interchange of Energy in/out of NC</t>
+  </si>
+  <si>
+    <t>#ffdf09</t>
+  </si>
+  <si>
+    <t>#f0fd1f</t>
+  </si>
+  <si>
+    <t>#b9ff2c</t>
   </si>
 </sst>
 </file>
@@ -870,7 +894,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="43">
+  <fills count="44">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1107,6 +1131,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1614,7 +1644,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1637,6 +1667,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="344">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2295,7 +2335,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -2311,7 +2351,7 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2349,10 +2389,10 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -2363,10 +2403,10 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
@@ -2377,10 +2417,10 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B4" t="s">
         <v>161</v>
-      </c>
-      <c r="B4" t="s">
-        <v>162</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>
@@ -2391,10 +2431,10 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
@@ -2405,10 +2445,10 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
@@ -2419,10 +2459,10 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C7" t="s">
         <v>18</v>
@@ -2433,10 +2473,10 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C8" t="s">
         <v>65</v>
@@ -2447,10 +2487,10 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C9" t="s">
         <v>65</v>
@@ -2461,10 +2501,10 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C10" t="s">
         <v>65</v>
@@ -2483,8 +2523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C5C9527-1881-4D6D-BD71-38E11E56DCAB}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44:D64"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2513,7 +2553,7 @@
         <v>2023</v>
       </c>
       <c r="B2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C2" s="1">
         <v>9.5000000000000001E-2</v>
@@ -2527,7 +2567,7 @@
         <v>2025</v>
       </c>
       <c r="B3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C3" s="1">
         <v>9.5000000000000001E-2</v>
@@ -2541,7 +2581,7 @@
         <v>2030</v>
       </c>
       <c r="B4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C4" s="1">
         <v>9.5000000000000001E-2</v>
@@ -2555,7 +2595,7 @@
         <v>2035</v>
       </c>
       <c r="B5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C5" s="1">
         <v>9.5000000000000001E-2</v>
@@ -2569,7 +2609,7 @@
         <v>2040</v>
       </c>
       <c r="B6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C6" s="1">
         <v>9.5000000000000001E-2</v>
@@ -2583,7 +2623,7 @@
         <v>2045</v>
       </c>
       <c r="B7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C7" s="1">
         <v>9.5000000000000001E-2</v>
@@ -2597,7 +2637,7 @@
         <v>2050</v>
       </c>
       <c r="B8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C8" s="1">
         <v>9.5000000000000001E-2</v>
@@ -2611,7 +2651,7 @@
         <v>2023</v>
       </c>
       <c r="B9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C9" s="1">
         <v>2.0579999999999998</v>
@@ -2625,7 +2665,7 @@
         <v>2025</v>
       </c>
       <c r="B10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C10" s="1">
         <v>2.0579999999999998</v>
@@ -2639,7 +2679,7 @@
         <v>2030</v>
       </c>
       <c r="B11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C11" s="1">
         <v>2.0579999999999998</v>
@@ -2653,7 +2693,7 @@
         <v>2035</v>
       </c>
       <c r="B12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C12" s="1">
         <v>2.0579999999999998</v>
@@ -2667,7 +2707,7 @@
         <v>2040</v>
       </c>
       <c r="B13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C13" s="1">
         <v>2.0579999999999998</v>
@@ -2681,7 +2721,7 @@
         <v>2045</v>
       </c>
       <c r="B14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C14" s="1">
         <v>2.0579999999999998</v>
@@ -2695,7 +2735,7 @@
         <v>2050</v>
       </c>
       <c r="B15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C15" s="1">
         <v>2.0579999999999998</v>
@@ -2709,13 +2749,13 @@
         <v>2023</v>
       </c>
       <c r="B16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C16" s="1">
         <v>0</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -2723,13 +2763,13 @@
         <v>2025</v>
       </c>
       <c r="B17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C17" s="1">
         <v>0</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2737,13 +2777,13 @@
         <v>2030</v>
       </c>
       <c r="B18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C18" s="1">
         <v>0</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -2751,13 +2791,13 @@
         <v>2035</v>
       </c>
       <c r="B19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C19" s="1">
         <v>0</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -2765,13 +2805,13 @@
         <v>2040</v>
       </c>
       <c r="B20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C20" s="1">
         <v>0</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2779,13 +2819,13 @@
         <v>2045</v>
       </c>
       <c r="B21" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C21" s="1">
         <v>0</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -2793,13 +2833,13 @@
         <v>2050</v>
       </c>
       <c r="B22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C22" s="1">
         <v>0</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2807,13 +2847,13 @@
         <v>2023</v>
       </c>
       <c r="B23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C23" s="1">
         <v>0</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -2821,13 +2861,13 @@
         <v>2025</v>
       </c>
       <c r="B24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C24" s="1">
         <v>0</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2835,13 +2875,13 @@
         <v>2030</v>
       </c>
       <c r="B25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C25" s="1">
         <v>0</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -2849,13 +2889,13 @@
         <v>2035</v>
       </c>
       <c r="B26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C26" s="1">
         <v>0</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -2863,13 +2903,13 @@
         <v>2040</v>
       </c>
       <c r="B27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C27" s="1">
         <v>0</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -2877,13 +2917,13 @@
         <v>2045</v>
       </c>
       <c r="B28" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C28" s="1">
         <v>0</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -2891,13 +2931,13 @@
         <v>2050</v>
       </c>
       <c r="B29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C29" s="1">
         <v>0</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -2905,13 +2945,13 @@
         <v>2023</v>
       </c>
       <c r="B30" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C30" s="1">
         <v>0</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -2919,13 +2959,13 @@
         <v>2025</v>
       </c>
       <c r="B31" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C31" s="1">
         <v>0</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -2933,13 +2973,13 @@
         <v>2030</v>
       </c>
       <c r="B32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C32" s="1">
         <v>0</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -2947,13 +2987,13 @@
         <v>2035</v>
       </c>
       <c r="B33" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C33" s="1">
         <v>0</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -2961,13 +3001,13 @@
         <v>2040</v>
       </c>
       <c r="B34" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C34" s="1">
         <v>0</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -2975,13 +3015,13 @@
         <v>2045</v>
       </c>
       <c r="B35" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C35" s="1">
         <v>0</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -2989,13 +3029,13 @@
         <v>2050</v>
       </c>
       <c r="B36" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C36" s="1">
         <v>0</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -3003,13 +3043,13 @@
         <v>2023</v>
       </c>
       <c r="B37" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C37" s="1">
         <v>0</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -3017,13 +3057,13 @@
         <v>2025</v>
       </c>
       <c r="B38" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C38" s="1">
         <v>0</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -3031,13 +3071,13 @@
         <v>2030</v>
       </c>
       <c r="B39" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C39" s="1">
         <v>0</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -3045,13 +3085,13 @@
         <v>2035</v>
       </c>
       <c r="B40" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C40" s="1">
         <v>0</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -3059,13 +3099,13 @@
         <v>2040</v>
       </c>
       <c r="B41" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C41" s="1">
         <v>0</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -3073,13 +3113,13 @@
         <v>2045</v>
       </c>
       <c r="B42" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C42" s="1">
         <v>0</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -3087,13 +3127,13 @@
         <v>2050</v>
       </c>
       <c r="B43" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C43" s="1">
         <v>0</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -3101,13 +3141,13 @@
         <v>2023</v>
       </c>
       <c r="B44" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C44" s="1">
         <v>0.85</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -3115,13 +3155,13 @@
         <v>2025</v>
       </c>
       <c r="B45" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C45" s="1">
         <v>0.85</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -3129,13 +3169,13 @@
         <v>2030</v>
       </c>
       <c r="B46" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C46" s="1">
         <v>0.85</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -3143,13 +3183,13 @@
         <v>2035</v>
       </c>
       <c r="B47" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C47" s="1">
         <v>0.85</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -3157,13 +3197,13 @@
         <v>2040</v>
       </c>
       <c r="B48" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C48" s="1">
         <v>0.85</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -3171,13 +3211,13 @@
         <v>2045</v>
       </c>
       <c r="B49" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C49" s="1">
         <v>0.85</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -3185,13 +3225,13 @@
         <v>2050</v>
       </c>
       <c r="B50" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C50" s="1">
         <v>0.85</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -3199,13 +3239,13 @@
         <v>2023</v>
       </c>
       <c r="B51" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C51" s="1">
         <v>4.07</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -3213,13 +3253,13 @@
         <v>2025</v>
       </c>
       <c r="B52" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C52" s="1">
         <v>4.07</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -3227,13 +3267,13 @@
         <v>2030</v>
       </c>
       <c r="B53" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C53" s="1">
         <v>4.07</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -3241,13 +3281,13 @@
         <v>2035</v>
       </c>
       <c r="B54" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C54" s="1">
         <v>4.07</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -3255,13 +3295,13 @@
         <v>2040</v>
       </c>
       <c r="B55" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C55" s="1">
         <v>4.07</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -3269,13 +3309,13 @@
         <v>2045</v>
       </c>
       <c r="B56" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C56" s="1">
         <v>4.07</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -3283,13 +3323,13 @@
         <v>2050</v>
       </c>
       <c r="B57" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C57" s="1">
         <v>4.07</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -3297,13 +3337,13 @@
         <v>2023</v>
       </c>
       <c r="B58" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C58" s="1">
         <v>11</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -3311,13 +3351,13 @@
         <v>2025</v>
       </c>
       <c r="B59" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C59" s="1">
         <v>11</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -3325,13 +3365,13 @@
         <v>2030</v>
       </c>
       <c r="B60" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C60" s="1">
         <v>11</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -3339,13 +3379,13 @@
         <v>2035</v>
       </c>
       <c r="B61" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C61" s="1">
         <v>11</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -3353,13 +3393,13 @@
         <v>2040</v>
       </c>
       <c r="B62" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C62" s="1">
         <v>11</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -3367,13 +3407,13 @@
         <v>2045</v>
       </c>
       <c r="B63" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C63" s="1">
         <v>11</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -3381,13 +3421,13 @@
         <v>2050</v>
       </c>
       <c r="B64" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C64" s="1">
         <v>11</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -3398,10 +3438,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB0F5A9-D905-4459-BBED-C585707C2B23}">
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3638,11 +3678,11 @@
       <c r="A17" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="C17" s="8">
-        <v>11</v>
+      <c r="B17" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="C17" s="14">
+        <v>-1</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>92</v>
@@ -3695,7 +3735,7 @@
         <v>42</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C21" s="10">
         <v>11</v>
@@ -3709,7 +3749,7 @@
         <v>43</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C22" s="11">
         <v>6</v>
@@ -3970,31 +4010,31 @@
         <v>115</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
-      <c r="A41" t="s">
-        <v>62</v>
-      </c>
-      <c r="B41" t="s">
-        <v>25</v>
-      </c>
-      <c r="C41">
-        <v>19</v>
-      </c>
-      <c r="D41" t="s">
+    <row r="41" spans="1:4" s="14" customFormat="1">
+      <c r="A41" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="C41" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D41" s="14" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
-      <c r="A42" t="s">
-        <v>63</v>
-      </c>
-      <c r="B42" t="s">
-        <v>25</v>
-      </c>
-      <c r="C42">
-        <v>0</v>
-      </c>
-      <c r="D42" t="s">
+    <row r="42" spans="1:4" s="14" customFormat="1">
+      <c r="A42" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="C42" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D42" s="14" t="s">
         <v>117</v>
       </c>
     </row>
@@ -4196,128 +4236,156 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B57" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C57">
         <v>0</v>
       </c>
       <c r="D57" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B58" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C58">
         <v>1</v>
       </c>
       <c r="D58" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B59" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C59">
         <v>2</v>
       </c>
       <c r="D59" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B60" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C60">
         <v>3</v>
       </c>
       <c r="D60" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B61" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C61">
         <v>4</v>
       </c>
       <c r="D61" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B62" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C62">
         <v>5</v>
       </c>
       <c r="D62" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B63" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C63">
         <v>6</v>
       </c>
       <c r="D63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B64" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C64">
         <v>7</v>
       </c>
       <c r="D64" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B65" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C65">
         <v>8</v>
       </c>
       <c r="D65" t="s">
-        <v>157</v>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" t="s">
+        <v>179</v>
+      </c>
+      <c r="B66" t="s">
+        <v>25</v>
+      </c>
+      <c r="C66">
+        <v>7</v>
+      </c>
+      <c r="D66" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" t="s">
+        <v>180</v>
+      </c>
+      <c r="B67" t="s">
+        <v>25</v>
+      </c>
+      <c r="C67">
+        <v>7</v>
+      </c>
+      <c r="D67" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -4330,8 +4398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3D25B83-BD09-4826-A0C5-07C0037AF25E}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4343,34 +4411,34 @@
   <sheetData>
     <row r="1" spans="1:10" s="12" customFormat="1">
       <c r="A1" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="H1" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="D1" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="H1" s="12" t="s">
+      <c r="I1" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="I1" s="12" t="s">
-        <v>153</v>
-      </c>
       <c r="J1" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -4409,9 +4477,15 @@
       <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
+      <c r="B3" s="16" t="s">
+        <v>60</v>
+      </c>
       <c r="C3" t="s">
         <v>36</v>
       </c>
+      <c r="D3" s="18" t="s">
+        <v>50</v>
+      </c>
       <c r="E3" t="s">
         <v>29</v>
       </c>
@@ -4420,6 +4494,12 @@
       </c>
       <c r="G3" t="s">
         <v>20</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="I3" s="22" t="s">
+        <v>65</v>
       </c>
       <c r="J3" s="13" t="s">
         <v>27</v>
@@ -4429,11 +4509,29 @@
       <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
+      <c r="B4" s="16" t="s">
+        <v>61</v>
+      </c>
       <c r="C4" t="s">
         <v>37</v>
       </c>
+      <c r="D4" s="18" t="s">
+        <v>51</v>
+      </c>
       <c r="E4" t="s">
         <v>30</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="I4" s="22" t="s">
+        <v>66</v>
       </c>
       <c r="J4" t="s">
         <v>31</v>
@@ -4443,6 +4541,21 @@
       <c r="A5" s="12" t="s">
         <v>4</v>
       </c>
+      <c r="C5" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>64</v>
+      </c>
       <c r="J5" t="s">
         <v>32</v>
       </c>
@@ -4451,6 +4564,12 @@
       <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
+      <c r="C6" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>46</v>
+      </c>
       <c r="J6" t="s">
         <v>39</v>
       </c>
@@ -4459,6 +4578,12 @@
       <c r="A7" s="12" t="s">
         <v>6</v>
       </c>
+      <c r="C7" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>47</v>
+      </c>
       <c r="J7" t="s">
         <v>41</v>
       </c>
@@ -4467,6 +4592,9 @@
       <c r="A8" s="12" t="s">
         <v>7</v>
       </c>
+      <c r="C8" s="19" t="s">
+        <v>56</v>
+      </c>
       <c r="J8" t="s">
         <v>42</v>
       </c>
@@ -4475,65 +4603,80 @@
       <c r="A9" s="12" t="s">
         <v>8</v>
       </c>
+      <c r="C9" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="J9" s="17" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="12" t="s">
         <v>9</v>
       </c>
+      <c r="C10" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="J10" s="17" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="12" t="s">
         <v>10</v>
       </c>
+      <c r="C11" s="19" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -4546,7 +4689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0978FAC-F8A3-4A10-8299-10A36FF1B366}">
   <dimension ref="A1:A56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
@@ -4557,7 +4700,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:1">

</xml_diff>

<commit_message>
Added Retrofit NG and Coal
</commit_message>
<xml_diff>
--- a/CreateDB_NC/InputData/ExcelUserData/UserDataPart3.xlsx
+++ b/CreateDB_NC/InputData/ExcelUserData/UserDataPart3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Remote\Desktop\Projects\TemoaHurricane_OEA\TEMOA_GIT\TemoaHurricane_V2\CreateDB_NC\InputData\ExcelUserData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{528B3737-44F8-40F0-91F5-7723DB5ABBAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BEA1EBE-B289-4BC5-B8C8-60AAF9711E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="200">
   <si>
     <t>Group Name</t>
   </si>
@@ -598,6 +598,48 @@
   </si>
   <si>
     <t>#b9ff2c</t>
+  </si>
+  <si>
+    <t>NG_F-FRAME_CC_NEW_NO_RFIT</t>
+  </si>
+  <si>
+    <t>NG_F-FRAME_CT_NEW_NO_RFIT</t>
+  </si>
+  <si>
+    <t>NG_H-FRAME_CC_NEW_NO_RFIT</t>
+  </si>
+  <si>
+    <t>COAL_NEW_NO_RFIT</t>
+  </si>
+  <si>
+    <t>NG_F-FRAME_CC_NEW_RFIT</t>
+  </si>
+  <si>
+    <t>NG_F-FRAME_CT_NEW_RFIT</t>
+  </si>
+  <si>
+    <t>NG_H-FRAME_CC_NEW_RFIT</t>
+  </si>
+  <si>
+    <t>COAL_NEW_RFIT</t>
+  </si>
+  <si>
+    <t>NG_CC_EX_NO_RFIT</t>
+  </si>
+  <si>
+    <t>NG_GT_EX_NO_RFIT</t>
+  </si>
+  <si>
+    <t>BIT_ST_EX_NO_RFIT</t>
+  </si>
+  <si>
+    <t>NG_CC_EX_RFIT</t>
+  </si>
+  <si>
+    <t>NG_GT_EX_RFIT</t>
+  </si>
+  <si>
+    <t>BIT_ST_EX_RFIT</t>
   </si>
 </sst>
 </file>
@@ -894,7 +936,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="44">
+  <fills count="45">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1137,6 +1179,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1644,7 +1692,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1668,15 +1716,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="344">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2523,7 +2563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C5C9527-1881-4D6D-BD71-38E11E56DCAB}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -3438,15 +3478,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB0F5A9-D905-4459-BBED-C585707C2B23}">
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68:A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="41.28515625" customWidth="1"/>
+    <col min="2" max="3" width="22.140625" customWidth="1"/>
     <col min="4" max="4" width="82.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4386,6 +4427,160 @@
       </c>
       <c r="D67" t="s">
         <v>182</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" s="15" customFormat="1">
+      <c r="A68" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="B68" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C68" s="15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" s="15" customFormat="1">
+      <c r="A69" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="B69" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C69" s="15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" s="15" customFormat="1">
+      <c r="A70" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="B70" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C70" s="15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" s="15" customFormat="1">
+      <c r="A71" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="B71" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C71" s="15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" s="15" customFormat="1">
+      <c r="A72" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="B72" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C72" s="15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" s="15" customFormat="1">
+      <c r="A73" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="B73" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C73" s="15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" s="15" customFormat="1">
+      <c r="A74" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="B74" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C74" s="15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" s="15" customFormat="1">
+      <c r="A75" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="B75" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C75" s="15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" s="15" customFormat="1">
+      <c r="A76" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="B76" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C76" s="15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" s="15" customFormat="1">
+      <c r="A77" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="B77" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C77" s="15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" s="15" customFormat="1">
+      <c r="A78" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="B78" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C78" s="15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" s="15" customFormat="1">
+      <c r="A79" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B79" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C79" s="15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" s="15" customFormat="1">
+      <c r="A80" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="B80" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C80" s="15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" s="15" customFormat="1">
+      <c r="A81" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="B81" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C81" s="15">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -4399,13 +4594,15 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="10" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" customWidth="1"/>
+    <col min="4" max="10" width="20.85546875" customWidth="1"/>
     <col min="13" max="19" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4477,13 +4674,13 @@
       <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" t="s">
         <v>60</v>
       </c>
       <c r="C3" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" t="s">
         <v>50</v>
       </c>
       <c r="E3" t="s">
@@ -4495,10 +4692,10 @@
       <c r="G3" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" t="s">
         <v>177</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I3" t="s">
         <v>65</v>
       </c>
       <c r="J3" s="13" t="s">
@@ -4509,28 +4706,28 @@
       <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" t="s">
         <v>61</v>
       </c>
       <c r="C4" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" t="s">
         <v>51</v>
       </c>
       <c r="E4" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" t="s">
         <v>178</v>
       </c>
-      <c r="I4" s="22" t="s">
+      <c r="I4" t="s">
         <v>66</v>
       </c>
       <c r="J4" t="s">
@@ -4541,19 +4738,19 @@
       <c r="A5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="21" t="s">
+      <c r="G5" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="H5" t="s">
         <v>64</v>
       </c>
       <c r="J5" t="s">
@@ -4564,10 +4761,10 @@
       <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" t="s">
         <v>54</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" t="s">
         <v>46</v>
       </c>
       <c r="J6" t="s">
@@ -4578,10 +4775,10 @@
       <c r="A7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" t="s">
         <v>55</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" t="s">
         <v>47</v>
       </c>
       <c r="J7" t="s">
@@ -4592,7 +4789,7 @@
       <c r="A8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" t="s">
         <v>56</v>
       </c>
       <c r="J8" t="s">
@@ -4603,10 +4800,10 @@
       <c r="A9" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" t="s">
         <v>57</v>
       </c>
-      <c r="J9" s="17" t="s">
+      <c r="J9" t="s">
         <v>48</v>
       </c>
     </row>
@@ -4614,10 +4811,10 @@
       <c r="A10" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" t="s">
         <v>58</v>
       </c>
-      <c r="J10" s="17" t="s">
+      <c r="J10" t="s">
         <v>49</v>
       </c>
     </row>
@@ -4625,7 +4822,7 @@
       <c r="A11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" t="s">
         <v>59</v>
       </c>
     </row>
@@ -4687,10 +4884,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0978FAC-F8A3-4A10-8299-10A36FF1B366}">
-  <dimension ref="A1:A56"/>
+  <dimension ref="A1:A72"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59:A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4978,6 +5175,86 @@
         <v>75</v>
       </c>
     </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
+        <v>193</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>